<commit_message>
update camas h. SE34
</commit_message>
<xml_diff>
--- a/data/source1_camas/input/disponibilidad_camas_hospitalarias.xlsx
+++ b/data/source1_camas/input/disponibilidad_camas_hospitalarias.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\GitHub\covid-cusco\dashboard-covid-geresa\data\source1_camas\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{046A95F1-D688-4936-8554-954226C29344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDD00710-32F8-477A-971A-1C35AA436B40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="384" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -109,7 +109,28 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -385,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E418"/>
+  <dimension ref="A1:E425"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A392" workbookViewId="0">
-      <selection activeCell="D418" sqref="D418"/>
+    <sheetView tabSelected="1" topLeftCell="A398" workbookViewId="0">
+      <selection activeCell="A418" sqref="A418:A425"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6407,6 +6428,125 @@
         <v>0.64</v>
       </c>
     </row>
+    <row r="419" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A419" s="1">
+        <v>44430</v>
+      </c>
+      <c r="B419">
+        <v>1</v>
+      </c>
+      <c r="C419">
+        <v>0.16483516483516483</v>
+      </c>
+      <c r="D419">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="E419">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="420" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A420" s="1">
+        <v>44431</v>
+      </c>
+      <c r="B420">
+        <v>1</v>
+      </c>
+      <c r="C420">
+        <v>0.1650943396226415</v>
+      </c>
+      <c r="D420">
+        <v>0.10843373493975904</v>
+      </c>
+      <c r="E420">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="421" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A421" s="1">
+        <v>44432</v>
+      </c>
+      <c r="B421">
+        <v>0.94871794871794868</v>
+      </c>
+      <c r="C421">
+        <v>0.16981132075471697</v>
+      </c>
+      <c r="D421">
+        <v>0.11244979919678715</v>
+      </c>
+      <c r="E421">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="422" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A422" s="1">
+        <v>44433</v>
+      </c>
+      <c r="B422">
+        <v>0.94871794871794868</v>
+      </c>
+      <c r="C422">
+        <v>0.15748031496062992</v>
+      </c>
+      <c r="D422">
+        <v>0.11693548387096774</v>
+      </c>
+      <c r="E422">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="423" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A423" s="1">
+        <v>44434</v>
+      </c>
+      <c r="B423">
+        <v>0.94871794871794868</v>
+      </c>
+      <c r="C423">
+        <v>0.17637795275590551</v>
+      </c>
+      <c r="D423">
+        <v>0.10887096774193548</v>
+      </c>
+      <c r="E423">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="424" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A424" s="1">
+        <v>44435</v>
+      </c>
+      <c r="B424">
+        <v>0.97435897435897434</v>
+      </c>
+      <c r="C424">
+        <v>0.17535545023696683</v>
+      </c>
+      <c r="D424">
+        <v>0.10975609756097561</v>
+      </c>
+      <c r="E424">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="425" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A425" s="1">
+        <v>44436</v>
+      </c>
+      <c r="B425">
+        <v>0.97435897435897434</v>
+      </c>
+      <c r="C425">
+        <v>0.17535545023696683</v>
+      </c>
+      <c r="D425">
+        <v>0.10975609756097561</v>
+      </c>
+      <c r="E425">
+        <v>0.36</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>